<commit_message>
update instances (add a prescription for infusion and 3 separates prescriptions) f06a5661a8791101015cdb6e446af49a656cbff9
</commit_message>
<xml_diff>
--- a/update_instances/ig/CodeSystem-CSMedications.xlsx
+++ b/update_instances/ig/CodeSystem-CSMedications.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-27T14:24:55+00:00</t>
+    <t>2024-03-27T14:30:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -114,7 +114,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>12</t>
+    <t>9</t>
   </si>
   <si>
     <t>Level</t>
@@ -172,24 +172,6 @@
   </si>
   <si>
     <t>OXYCODONE LP 10 MG VIATRIS, CPR À LIBÉRATION PROLONGÉE</t>
-  </si>
-  <si>
-    <t>9075933</t>
-  </si>
-  <si>
-    <t>PROFENID 50 MG, GÉLULE</t>
-  </si>
-  <si>
-    <t>3400892028057</t>
-  </si>
-  <si>
-    <t>DOLIPRANE 2,4% BUV SS SUCRE FL 100ML</t>
-  </si>
-  <si>
-    <t>9100298</t>
-  </si>
-  <si>
-    <t>VIT B12 DEL 1MG/2ML INJ BUV AMP</t>
   </si>
   <si>
     <t>9009043</t>
@@ -506,7 +488,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -634,42 +616,6 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>